<commit_message>
oil and gas companies added
</commit_message>
<xml_diff>
--- a/twitter-queries/marktaandelen.xlsx
+++ b/twitter-queries/marktaandelen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Consoles" sheetId="3" r:id="rId1"/>
@@ -7488,7 +7488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -7774,8 +7774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>

</xml_diff>